<commit_message>
Slideshow can now generate a list of slides from an Excel doc.
</commit_message>
<xml_diff>
--- a/UnitTests/TestFile.xlsx
+++ b/UnitTests/TestFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Slide Number</t>
   </si>
@@ -35,13 +35,7 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Disabled</t>
-  </si>
-  <si>
     <t>Enabled?</t>
-  </si>
-  <si>
-    <t>Enabled</t>
   </si>
   <si>
     <t>Testing</t>
@@ -365,7 +359,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="A6:D6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +379,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -393,13 +387,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="D2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -410,10 +404,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -424,10 +418,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -440,8 +434,8 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>3</v>
+      <c r="D5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>